<commit_message>
remove internal error during reading s7 tags
</commit_message>
<xml_diff>
--- a/Snap7/src/tags/s7-tags-s1-p2.xlsx
+++ b/Snap7/src/tags/s7-tags-s1-p2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbystrzycki\Desktop\Snap7\src\tags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19544BD7-49F5-421E-A16D-400F0ADC7E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02681EB-D2B6-4AA9-BE1C-D0C5B06BA310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S7-Tags" sheetId="25" r:id="rId1"/>
@@ -666,7 +666,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +731,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="1">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -754,19 +754,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E5" s="3">
         <v>310</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
@@ -789,10 +789,10 @@
         <v>306</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="1"/>
@@ -809,7 +809,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="3">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E7" s="3">
         <v>34</v>
@@ -835,7 +835,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="1">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E8" s="1">
         <v>38</v>

</xml_diff>

<commit_message>
s7 tags with id
</commit_message>
<xml_diff>
--- a/Snap7/src/tags/s7-tags-s1-p2.xlsx
+++ b/Snap7/src/tags/s7-tags-s1-p2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbystrzycki\Desktop\Snap7\src\tags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02681EB-D2B6-4AA9-BE1C-D0C5B06BA310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7AD928-046B-417C-A161-0FD8387E1E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -666,7 +666,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +731,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="1">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -754,19 +754,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="3">
         <v>310</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
@@ -792,7 +792,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="1"/>
@@ -809,7 +809,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="3">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" s="3">
         <v>34</v>
@@ -835,7 +835,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="1">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E8" s="1">
         <v>38</v>

</xml_diff>